<commit_message>
changes to recalculate subject marks
</commit_message>
<xml_diff>
--- a/a-results3.xlsx
+++ b/a-results3.xlsx
@@ -748,34 +748,34 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>68.66666666666667</v>
+        <v>103</v>
       </c>
       <c r="D10" t="n">
-        <v>62.33333333333334</v>
+        <v>93.5</v>
       </c>
       <c r="E10" t="n">
-        <v>51.33333333333334</v>
+        <v>77</v>
       </c>
       <c r="F10" t="n">
-        <v>55.66666666666666</v>
+        <v>83.5</v>
       </c>
       <c r="G10" t="n">
-        <v>82.33333333333333</v>
+        <v>123.5</v>
       </c>
       <c r="H10" t="n">
-        <v>68.33333333333333</v>
+        <v>102.5</v>
       </c>
       <c r="I10" t="n">
-        <v>52.66666666666666</v>
+        <v>79</v>
       </c>
       <c r="J10" t="n">
-        <v>81.33333333333333</v>
+        <v>122</v>
       </c>
       <c r="K10" t="n">
-        <v>522.6666666666666</v>
+        <v>784</v>
       </c>
       <c r="L10" t="n">
-        <v>65.33333333333333</v>
+        <v>98</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -796,42 +796,42 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>C+</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>C-</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>C-</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>A-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">

</xml_diff>